<commit_message>
working with cs dataset
</commit_message>
<xml_diff>
--- a/MAD/gt_workdir/cs_annotation.xlsx
+++ b/MAD/gt_workdir/cs_annotation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\mad_project\MAD\gt_workdir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF4DD060-C0DA-40E3-8373-32229B348E97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12FBE14B-8ED1-4015-961D-7D1F28D84EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B35E8438-7317-4408-9CEC-581174F07A90}"/>
   </bookViews>
@@ -28,8 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>video name</t>
   </si>
@@ -60,69 +58,6 @@
     <t>framerate</t>
   </si>
   <si>
-    <t>/content/drive/MyDrive/VAD_Code/VAD_Code/normal_fea_new/Normal_Videos_129_x264.mp4.npy</t>
-  </si>
-  <si>
-    <t>/content/drive/MyDrive/VAD_Code/VAD_Code/normal_fea_new/Normal_Videos_150_x264.mp4.npy</t>
-  </si>
-  <si>
-    <t>/content/drive/MyDrive/VAD_Code/VAD_Code/normal_fea_new/Normal_Videos_246_x264.mp4.npy</t>
-  </si>
-  <si>
-    <t>/content/drive/MyDrive/VAD_Code/VAD_Code/normal_fea_new/Normal_Videos_247_x264.mp4.npy</t>
-  </si>
-  <si>
-    <t>/content/drive/MyDrive/VAD_Code/VAD_Code/normal_fea_new/Normal_Videos_015_x264.npy</t>
-  </si>
-  <si>
-    <t>/content/drive/MyDrive/VAD_Code/VAD_Code/normal_fea_new/Normal_Videos_050_x264.npy</t>
-  </si>
-  <si>
-    <t>/content/drive/MyDrive/VAD_Code/VAD_Code/normal_fea_new/Normal_Videos_100_x264.npy</t>
-  </si>
-  <si>
-    <t>/content/drive/MyDrive/VAD_Code/VAD_Code/normal_fea_new/Normal_Videos_248_x264.npy</t>
-  </si>
-  <si>
-    <t>/content/drive/MyDrive/VAD_Code/VAD_Code/normal_fea_new/Normal_Videos_251_x264.npy</t>
-  </si>
-  <si>
-    <t>/content/drive/MyDrive/VAD_Code/VAD_Code/normal_fea_new/Normal_Videos_289_x264.npy</t>
-  </si>
-  <si>
-    <t>/content/drive/MyDrive/VAD_Code/VAD_Code/normal_fea_new/Normal_Videos_310_x264.npy</t>
-  </si>
-  <si>
-    <t>/content/drive/MyDrive/VAD_Code/VAD_Code/normal_fea_new/Normal_Videos_312_x264.npy</t>
-  </si>
-  <si>
-    <t>/content/drive/MyDrive/VAD_Code/VAD_Code/normal_fea_new/Normal_Videos_317_x264.npy</t>
-  </si>
-  <si>
-    <t>/content/drive/MyDrive/VAD_Code/VAD_Code/normal_fea_new/Normal_Videos_345_x264.npy</t>
-  </si>
-  <si>
-    <t>/content/drive/MyDrive/VAD_Code/VAD_Code/normal_fea_new/Normal_Videos_352_x264.npy</t>
-  </si>
-  <si>
-    <t>/content/drive/MyDrive/VAD_Code/VAD_Code/normal_fea_new/Normal_Videos_360_x264.npy</t>
-  </si>
-  <si>
-    <t>/content/drive/MyDrive/VAD_Code/VAD_Code/normal_fea_new/Normal_Videos_365_x264.npy</t>
-  </si>
-  <si>
-    <t>/content/drive/MyDrive/VAD_Code/VAD_Code/normal_fea_new/Normal_Videos_401_x264.npy</t>
-  </si>
-  <si>
-    <t>/content/drive/MyDrive/VAD_Code/VAD_Code/normal_fea_new/Normal_Videos_417_x264.npy</t>
-  </si>
-  <si>
-    <t>/content/drive/MyDrive/VAD_Code/VAD_Code/normal_fea_new/Normal_Videos_439_x264.npy</t>
-  </si>
-  <si>
-    <t>/mnt/c/code/data/fea_cs/</t>
-  </si>
-  <si>
     <t>/mnt/c/code/data/fea_cs/caught-on-cctv-khanna-woman-fights-off-chain-snatchers-bravely-1_3VIbwTFR (1).npy</t>
   </si>
   <si>
@@ -169,6 +104,66 @@
   </si>
   <si>
     <t>/mnt/c/code/data/fea_cs/watch-delhi-chain-snatching-govt-staffer-shoved-robbed-crime-on-cctv_ReApKPyA.npy</t>
+  </si>
+  <si>
+    <t>/mnt/c/code/data/fea_normal/Normal_Videos_015_x264.npy</t>
+  </si>
+  <si>
+    <t>/mnt/c/code/data/fea_normal/Normal_Videos_050_x264.npy</t>
+  </si>
+  <si>
+    <t>/mnt/c/code/data/fea_normal/Normal_Videos_100_x264.npy</t>
+  </si>
+  <si>
+    <t>/mnt/c/code/data/fea_normal/Normal_Videos_248_x264.npy</t>
+  </si>
+  <si>
+    <t>/mnt/c/code/data/fea_normal/Normal_Videos_251_x264.npy</t>
+  </si>
+  <si>
+    <t>/mnt/c/code/data/fea_normal/Normal_Videos_289_x264.npy</t>
+  </si>
+  <si>
+    <t>/mnt/c/code/data/fea_normal/Normal_Videos_310_x264.npy</t>
+  </si>
+  <si>
+    <t>/mnt/c/code/data/fea_normal/Normal_Videos_312_x264.npy</t>
+  </si>
+  <si>
+    <t>/mnt/c/code/data/fea_normal/Normal_Videos_317_x264.npy</t>
+  </si>
+  <si>
+    <t>/mnt/c/code/data/fea_normal/Normal_Videos_345_x264.npy</t>
+  </si>
+  <si>
+    <t>/mnt/c/code/data/fea_normal/Normal_Videos_352_x264.npy</t>
+  </si>
+  <si>
+    <t>/mnt/c/code/data/fea_normal/Normal_Videos_360_x264.npy</t>
+  </si>
+  <si>
+    <t>/mnt/c/code/data/fea_normal/Normal_Videos_365_x264.npy</t>
+  </si>
+  <si>
+    <t>/mnt/c/code/data/fea_normal/Normal_Videos_401_x264.npy</t>
+  </si>
+  <si>
+    <t>/mnt/c/code/data/fea_normal/Normal_Videos_417_x264.npy</t>
+  </si>
+  <si>
+    <t>/mnt/c/code/data/fea_normal/Normal_Videos_439_x264.npy</t>
+  </si>
+  <si>
+    <t>/mnt/c/code/data/fea_normal/Normal_Videos_129_x264.npy</t>
+  </si>
+  <si>
+    <t>/mnt/c/code/data/fea_normal/Normal_Videos_150_x264.npy</t>
+  </si>
+  <si>
+    <t>/mnt/c/code/data/fea_normal/Normal_Videos_246_x264.npy</t>
+  </si>
+  <si>
+    <t>/mnt/c/code/data/fea_normal/Normal_Videos_247_x264.npy</t>
   </si>
 </sst>
 </file>
@@ -523,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7564DCAB-DCA7-4F81-BCCA-E0C297E86A88}">
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -537,7 +532,7 @@
     <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -560,9 +555,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -585,9 +580,9 @@
         <v>625</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -610,9 +605,9 @@
         <v>330</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -634,13 +629,10 @@
         <f t="shared" si="1"/>
         <v>2000</v>
       </c>
-      <c r="K4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -663,9 +655,9 @@
         <v>400</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -688,9 +680,9 @@
         <v>624</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -713,9 +705,9 @@
         <v>300</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -738,9 +730,9 @@
         <v>2038.3</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -763,9 +755,9 @@
         <v>651.20000000000005</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -788,9 +780,9 @@
         <v>250</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -813,9 +805,9 @@
         <v>660</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -838,9 +830,9 @@
         <v>300</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -863,9 +855,9 @@
         <v>225</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -888,9 +880,9 @@
         <v>400</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -913,9 +905,9 @@
         <v>600</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -940,7 +932,7 @@
     </row>
     <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -963,9 +955,9 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B18" s="1">
         <v>0</v>
@@ -977,9 +969,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B19" s="1">
         <v>0</v>
@@ -991,9 +983,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B20" s="1">
         <v>0</v>
@@ -1005,9 +997,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="B21" s="1">
         <v>0</v>
@@ -1019,9 +1011,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="B22" s="1">
         <v>0</v>
@@ -1033,9 +1025,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="B23" s="1">
         <v>0</v>
@@ -1047,9 +1039,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="B24" s="1">
         <v>0</v>
@@ -1061,9 +1053,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B25" s="1">
         <v>0</v>
@@ -1075,9 +1067,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B26" s="1">
         <v>0</v>
@@ -1089,9 +1081,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B27" s="1">
         <v>0</v>
@@ -1103,9 +1095,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B28" s="1">
         <v>0</v>
@@ -1117,9 +1109,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B29" s="1">
         <v>0</v>
@@ -1131,9 +1123,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B30" s="1">
         <v>0</v>
@@ -1145,9 +1137,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B31" s="1">
         <v>0</v>
@@ -1159,9 +1151,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B32" s="1">
         <v>0</v>
@@ -1173,9 +1165,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B33" s="1">
         <v>0</v>
@@ -1187,9 +1179,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="B34" s="1">
         <v>0</v>
@@ -1201,9 +1193,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="B35" s="1">
         <v>0</v>
@@ -1215,9 +1207,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B36" s="1">
         <v>0</v>
@@ -1229,9 +1221,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B37" s="1">
         <v>0</v>

</xml_diff>